<commit_message>
Translated tabs names for report in ReportView, fixed Reporting Ratio tab title for events
</commit_message>
<xml_diff>
--- a/RShinyApps/mydata.xlsx
+++ b/RShinyApps/mydata.xlsx
@@ -17,7 +17,7 @@
     <t>Όνομα φαρμάκου</t>
   </si>
   <si>
-    <t>Μετρήσεις για NAUSEA</t>
+    <t>Μετρήσεις για FLUSHING</t>
   </si>
   <si>
     <t>PRR</t>
@@ -173,154 +173,154 @@
     <t>50</t>
   </si>
   <si>
-    <t>APREMILAST</t>
-  </si>
-  <si>
-    <t>ONDANSETRON HYDROCHLORIDE</t>
-  </si>
-  <si>
-    <t>DULOXETINE HYDROCHLORIDE</t>
+    <t>NIACIN</t>
   </si>
   <si>
     <t>DIMETHYL FUMARATE</t>
   </si>
   <si>
-    <t>LORAZEPAM</t>
+    <t>DALFAMPRIDINE</t>
+  </si>
+  <si>
+    <t>FISH OIL</t>
+  </si>
+  <si>
+    <t>ASPIRIN 325 MG</t>
+  </si>
+  <si>
+    <t>ASPIRIN 81MG</t>
+  </si>
+  <si>
+    <t>ASPIRIN 81 MG</t>
+  </si>
+  <si>
+    <t>TREPROSTINIL</t>
+  </si>
+  <si>
+    <t>ASPIRIN</t>
+  </si>
+  <si>
+    <t>BENADRYL</t>
+  </si>
+  <si>
+    <t>TADALAFIL</t>
+  </si>
+  <si>
+    <t>GLATIRAMER ACETATE</t>
+  </si>
+  <si>
+    <t>DIPHENHYDRAMINE HYDROCHLORIDE</t>
+  </si>
+  <si>
+    <t>SILDENAFIL CITRATE</t>
+  </si>
+  <si>
+    <t>AMBRISENTAN</t>
+  </si>
+  <si>
+    <t>BACLOFEN</t>
+  </si>
+  <si>
+    <t>ROSUVASTATIN CALCIUM</t>
+  </si>
+  <si>
+    <t>ERGOCALCIFEROL</t>
+  </si>
+  <si>
+    <t>LISINOPRIL</t>
+  </si>
+  <si>
+    <t>WARFARIN SODIUM</t>
+  </si>
+  <si>
+    <t>ATORVASTATIN CALCIUM</t>
+  </si>
+  <si>
+    <t>CLOPIDOGREL</t>
+  </si>
+  <si>
+    <t>SIMVASTATIN</t>
+  </si>
+  <si>
+    <t>METOPROLOL</t>
+  </si>
+  <si>
+    <t>METOPROLOL TARTRATE</t>
+  </si>
+  <si>
+    <t>CLOPIDOGREL BISULFATE</t>
+  </si>
+  <si>
+    <t>HYDROCHLOROTHIAZIDE</t>
   </si>
   <si>
     <t>LEVOTHYROXINE SODIUM</t>
   </si>
   <si>
-    <t>ERGOCALCIFEROL</t>
+    <t>INFLIXIMAB</t>
+  </si>
+  <si>
+    <t>ATENOLOL</t>
   </si>
   <si>
     <t>RANITIDINE HYDROCHLORIDE</t>
   </si>
   <si>
-    <t>ALPRAZOLAM</t>
-  </si>
-  <si>
     <t>IBUPROFEN</t>
   </si>
   <si>
-    <t>SERTRALINE HYDROCHLORIDE</t>
-  </si>
-  <si>
-    <t>CLONAZEPAM</t>
+    <t>IBUPROFEN TABLETS</t>
+  </si>
+  <si>
+    <t>IBUPFROFEN</t>
+  </si>
+  <si>
+    <t>IBUPROFEN 200 MG</t>
+  </si>
+  <si>
+    <t>IBUPROFEN 200MG</t>
+  </si>
+  <si>
+    <t>IBUPROFEN ORAL</t>
+  </si>
+  <si>
+    <t>METFORMIN</t>
   </si>
   <si>
     <t>ACETAMINOPHEN</t>
   </si>
   <si>
-    <t>IBUPFROFEN</t>
-  </si>
-  <si>
-    <t>IBUPROFEN 200 MG</t>
-  </si>
-  <si>
-    <t>IBUPROFEN 200MG</t>
-  </si>
-  <si>
-    <t>IBUPROFEN ORAL</t>
-  </si>
-  <si>
-    <t>IBUPROFEN TABLETS</t>
-  </si>
-  <si>
-    <t>PANTOPRAZOLE</t>
-  </si>
-  <si>
     <t>GABAPENTIN</t>
   </si>
   <si>
-    <t>METFORMIN</t>
-  </si>
-  <si>
     <t>METFORMIN ER 500 MG</t>
   </si>
   <si>
     <t>METFORMIN ER 750 MG</t>
   </si>
   <si>
-    <t>LISINOPRIL</t>
-  </si>
-  <si>
     <t>OMEPRAZOLE MAGNESIUM</t>
   </si>
   <si>
-    <t>ATENOLOL</t>
-  </si>
-  <si>
-    <t>ALBUTEROL SULFATE</t>
+    <t>AMLODIPINE</t>
   </si>
   <si>
     <t>OMEPRAZOLE</t>
   </si>
   <si>
-    <t>FOLIC ACID</t>
-  </si>
-  <si>
-    <t>METOPROLOL TARTRATE</t>
-  </si>
-  <si>
-    <t>ATORVASTATIN CALCIUM</t>
+    <t>ESOMEPRAZOLE MAGNESIUM</t>
+  </si>
+  <si>
+    <t>ESOMEPRAZOLE SODIUM</t>
+  </si>
+  <si>
+    <t>DEXAMETHASONE</t>
+  </si>
+  <si>
+    <t>FUROSEMIDE</t>
   </si>
   <si>
     <t>PREDNISONE</t>
-  </si>
-  <si>
-    <t>METOPROLOL</t>
-  </si>
-  <si>
-    <t>ADALIMUMAB</t>
-  </si>
-  <si>
-    <t>ESOMEPRAZOLE MAGNESIUM</t>
-  </si>
-  <si>
-    <t>ESOMEPRAZOLE SODIUM</t>
-  </si>
-  <si>
-    <t>ETANERCEPT</t>
-  </si>
-  <si>
-    <t>METHOTREXATE SODIUM</t>
-  </si>
-  <si>
-    <t>DEXAMETHASONE</t>
-  </si>
-  <si>
-    <t>METHOTREXATE</t>
-  </si>
-  <si>
-    <t>AMLODIPINE</t>
-  </si>
-  <si>
-    <t>ASPIRIN</t>
-  </si>
-  <si>
-    <t>ASPIRIN 325 MG</t>
-  </si>
-  <si>
-    <t>ASPIRIN 81 MG</t>
-  </si>
-  <si>
-    <t>ASPIRIN 81MG</t>
-  </si>
-  <si>
-    <t>FUROSEMIDE</t>
-  </si>
-  <si>
-    <t>SIMVASTATIN</t>
-  </si>
-  <si>
-    <t>DEXAMETHASONE 1.5 MG</t>
-  </si>
-  <si>
-    <t>PREGABALIN</t>
-  </si>
-  <si>
-    <t>CLOPIDOGREL BISULFATE</t>
   </si>
 </sst>
 </file>
@@ -391,10 +391,10 @@
         <v>53</v>
       </c>
       <c r="C2" t="n">
-        <v>15210.0</v>
+        <v>11032.0</v>
       </c>
       <c r="D2" t="n">
-        <v>3.74</v>
+        <v>53.45</v>
       </c>
     </row>
     <row r="3">
@@ -405,10 +405,10 @@
         <v>54</v>
       </c>
       <c r="C3" t="n">
-        <v>11707.0</v>
+        <v>13832.0</v>
       </c>
       <c r="D3" t="n">
-        <v>2.86</v>
+        <v>23.6</v>
       </c>
     </row>
     <row r="4">
@@ -419,10 +419,10 @@
         <v>55</v>
       </c>
       <c r="C4" t="n">
-        <v>12523.0</v>
+        <v>1780.0</v>
       </c>
       <c r="D4" t="n">
-        <v>2.36</v>
+        <v>6.27</v>
       </c>
     </row>
     <row r="5">
@@ -433,10 +433,10 @@
         <v>56</v>
       </c>
       <c r="C5" t="n">
-        <v>7576.0</v>
+        <v>2537.0</v>
       </c>
       <c r="D5" t="n">
-        <v>1.77</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="6">
@@ -447,10 +447,10 @@
         <v>57</v>
       </c>
       <c r="C6" t="n">
-        <v>8480.0</v>
+        <v>10709.0</v>
       </c>
       <c r="D6" t="n">
-        <v>1.69</v>
+        <v>4.95</v>
       </c>
     </row>
     <row r="7">
@@ -461,10 +461,10 @@
         <v>58</v>
       </c>
       <c r="C7" t="n">
-        <v>14144.0</v>
+        <v>10707.0</v>
       </c>
       <c r="D7" t="n">
-        <v>1.63</v>
+        <v>4.95</v>
       </c>
     </row>
     <row r="8">
@@ -475,10 +475,10 @@
         <v>59</v>
       </c>
       <c r="C8" t="n">
-        <v>12869.0</v>
+        <v>10709.0</v>
       </c>
       <c r="D8" t="n">
-        <v>1.55</v>
+        <v>4.94</v>
       </c>
     </row>
     <row r="9">
@@ -489,10 +489,10 @@
         <v>60</v>
       </c>
       <c r="C9" t="n">
-        <v>6376.0</v>
+        <v>1411.0</v>
       </c>
       <c r="D9" t="n">
-        <v>1.52</v>
+        <v>4.81</v>
       </c>
     </row>
     <row r="10">
@@ -503,10 +503,10 @@
         <v>61</v>
       </c>
       <c r="C10" t="n">
-        <v>8489.0</v>
+        <v>10847.0</v>
       </c>
       <c r="D10" t="n">
-        <v>1.48</v>
+        <v>4.75</v>
       </c>
     </row>
     <row r="11">
@@ -517,10 +517,10 @@
         <v>62</v>
       </c>
       <c r="C11" t="n">
-        <v>9149.0</v>
+        <v>1436.0</v>
       </c>
       <c r="D11" t="n">
-        <v>1.48</v>
+        <v>4.31</v>
       </c>
     </row>
     <row r="12">
@@ -531,10 +531,10 @@
         <v>63</v>
       </c>
       <c r="C12" t="n">
-        <v>6132.0</v>
+        <v>1826.0</v>
       </c>
       <c r="D12" t="n">
-        <v>1.44</v>
+        <v>3.79</v>
       </c>
     </row>
     <row r="13">
@@ -545,10 +545,10 @@
         <v>64</v>
       </c>
       <c r="C13" t="n">
-        <v>6321.0</v>
+        <v>1094.0</v>
       </c>
       <c r="D13" t="n">
-        <v>1.43</v>
+        <v>3.24</v>
       </c>
     </row>
     <row r="14">
@@ -559,10 +559,10 @@
         <v>65</v>
       </c>
       <c r="C14" t="n">
-        <v>11119.0</v>
+        <v>1880.0</v>
       </c>
       <c r="D14" t="n">
-        <v>1.41</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="15">
@@ -573,10 +573,10 @@
         <v>66</v>
       </c>
       <c r="C15" t="n">
-        <v>6614.0</v>
+        <v>1374.0</v>
       </c>
       <c r="D15" t="n">
-        <v>1.37</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="16">
@@ -587,10 +587,10 @@
         <v>67</v>
       </c>
       <c r="C16" t="n">
-        <v>6618.0</v>
+        <v>1640.0</v>
       </c>
       <c r="D16" t="n">
-        <v>1.37</v>
+        <v>2.76</v>
       </c>
     </row>
     <row r="17">
@@ -601,10 +601,10 @@
         <v>68</v>
       </c>
       <c r="C17" t="n">
-        <v>6618.0</v>
+        <v>1056.0</v>
       </c>
       <c r="D17" t="n">
-        <v>1.37</v>
+        <v>2.49</v>
       </c>
     </row>
     <row r="18">
@@ -615,10 +615,10 @@
         <v>69</v>
       </c>
       <c r="C18" t="n">
-        <v>6615.0</v>
+        <v>2338.0</v>
       </c>
       <c r="D18" t="n">
-        <v>1.37</v>
+        <v>2.47</v>
       </c>
     </row>
     <row r="19">
@@ -629,10 +629,10 @@
         <v>70</v>
       </c>
       <c r="C19" t="n">
-        <v>6673.0</v>
+        <v>3088.0</v>
       </c>
       <c r="D19" t="n">
-        <v>1.37</v>
+        <v>2.09</v>
       </c>
     </row>
     <row r="20">
@@ -643,10 +643,10 @@
         <v>71</v>
       </c>
       <c r="C20" t="n">
-        <v>5987.0</v>
+        <v>3416.0</v>
       </c>
       <c r="D20" t="n">
-        <v>1.35</v>
+        <v>2.04</v>
       </c>
     </row>
     <row r="21">
@@ -657,10 +657,10 @@
         <v>72</v>
       </c>
       <c r="C21" t="n">
-        <v>12058.0</v>
+        <v>1269.0</v>
       </c>
       <c r="D21" t="n">
-        <v>1.34</v>
+        <v>1.86</v>
       </c>
     </row>
     <row r="22">
@@ -671,10 +671,10 @@
         <v>73</v>
       </c>
       <c r="C22" t="n">
-        <v>9141.0</v>
+        <v>2037.0</v>
       </c>
       <c r="D22" t="n">
-        <v>1.32</v>
+        <v>1.85</v>
       </c>
     </row>
     <row r="23">
@@ -685,10 +685,10 @@
         <v>74</v>
       </c>
       <c r="C23" t="n">
-        <v>7940.0</v>
+        <v>2028.0</v>
       </c>
       <c r="D23" t="n">
-        <v>1.32</v>
+        <v>1.83</v>
       </c>
     </row>
     <row r="24">
@@ -699,10 +699,10 @@
         <v>75</v>
       </c>
       <c r="C24" t="n">
-        <v>7940.0</v>
+        <v>2781.0</v>
       </c>
       <c r="D24" t="n">
-        <v>1.32</v>
+        <v>1.83</v>
       </c>
     </row>
     <row r="25">
@@ -713,10 +713,10 @@
         <v>76</v>
       </c>
       <c r="C25" t="n">
-        <v>12352.0</v>
+        <v>2031.0</v>
       </c>
       <c r="D25" t="n">
-        <v>1.31</v>
+        <v>1.78</v>
       </c>
     </row>
     <row r="26">
@@ -727,10 +727,10 @@
         <v>77</v>
       </c>
       <c r="C26" t="n">
-        <v>16549.0</v>
+        <v>2202.0</v>
       </c>
       <c r="D26" t="n">
-        <v>1.31</v>
+        <v>1.75</v>
       </c>
     </row>
     <row r="27">
@@ -741,10 +741,10 @@
         <v>78</v>
       </c>
       <c r="C27" t="n">
-        <v>6039.0</v>
+        <v>2048.0</v>
       </c>
       <c r="D27" t="n">
-        <v>1.3</v>
+        <v>1.74</v>
       </c>
     </row>
     <row r="28">
@@ -755,10 +755,10 @@
         <v>79</v>
       </c>
       <c r="C28" t="n">
-        <v>7665.0</v>
+        <v>1263.0</v>
       </c>
       <c r="D28" t="n">
-        <v>1.26</v>
+        <v>1.74</v>
       </c>
     </row>
     <row r="29">
@@ -769,10 +769,10 @@
         <v>80</v>
       </c>
       <c r="C29" t="n">
-        <v>11524.0</v>
+        <v>2671.0</v>
       </c>
       <c r="D29" t="n">
-        <v>1.26</v>
+        <v>1.7</v>
       </c>
     </row>
     <row r="30">
@@ -783,10 +783,10 @@
         <v>81</v>
       </c>
       <c r="C30" t="n">
-        <v>7703.0</v>
+        <v>1627.0</v>
       </c>
       <c r="D30" t="n">
-        <v>1.24</v>
+        <v>1.66</v>
       </c>
     </row>
     <row r="31">
@@ -797,10 +797,10 @@
         <v>82</v>
       </c>
       <c r="C31" t="n">
-        <v>8705.0</v>
+        <v>1298.0</v>
       </c>
       <c r="D31" t="n">
-        <v>1.24</v>
+        <v>1.56</v>
       </c>
     </row>
     <row r="32">
@@ -811,10 +811,10 @@
         <v>83</v>
       </c>
       <c r="C32" t="n">
-        <v>7617.0</v>
+        <v>1179.0</v>
       </c>
       <c r="D32" t="n">
-        <v>1.23</v>
+        <v>1.56</v>
       </c>
     </row>
     <row r="33">
@@ -825,10 +825,10 @@
         <v>84</v>
       </c>
       <c r="C33" t="n">
-        <v>13168.0</v>
+        <v>1452.0</v>
       </c>
       <c r="D33" t="n">
-        <v>1.23</v>
+        <v>1.29</v>
       </c>
     </row>
     <row r="34">
@@ -839,10 +839,10 @@
         <v>85</v>
       </c>
       <c r="C34" t="n">
-        <v>7756.0</v>
+        <v>1058.0</v>
       </c>
       <c r="D34" t="n">
-        <v>1.22</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="35">
@@ -853,10 +853,10 @@
         <v>86</v>
       </c>
       <c r="C35" t="n">
-        <v>10683.0</v>
+        <v>1025.0</v>
       </c>
       <c r="D35" t="n">
-        <v>1.2</v>
+        <v>1.17</v>
       </c>
     </row>
     <row r="36">
@@ -867,10 +867,10 @@
         <v>87</v>
       </c>
       <c r="C36" t="n">
-        <v>8324.0</v>
+        <v>1025.0</v>
       </c>
       <c r="D36" t="n">
-        <v>1.2</v>
+        <v>1.17</v>
       </c>
     </row>
     <row r="37">
@@ -881,10 +881,10 @@
         <v>88</v>
       </c>
       <c r="C37" t="n">
-        <v>7867.0</v>
+        <v>1025.0</v>
       </c>
       <c r="D37" t="n">
-        <v>1.2</v>
+        <v>1.17</v>
       </c>
     </row>
     <row r="38">
@@ -895,10 +895,10 @@
         <v>89</v>
       </c>
       <c r="C38" t="n">
-        <v>7247.0</v>
+        <v>1025.0</v>
       </c>
       <c r="D38" t="n">
-        <v>1.19</v>
+        <v>1.17</v>
       </c>
     </row>
     <row r="39">
@@ -909,10 +909,10 @@
         <v>90</v>
       </c>
       <c r="C39" t="n">
-        <v>14986.0</v>
+        <v>1420.0</v>
       </c>
       <c r="D39" t="n">
-        <v>1.19</v>
+        <v>1.13</v>
       </c>
     </row>
     <row r="40">
@@ -923,10 +923,10 @@
         <v>91</v>
       </c>
       <c r="C40" t="n">
-        <v>8067.0</v>
+        <v>1559.0</v>
       </c>
       <c r="D40" t="n">
-        <v>1.13</v>
+        <v>1.08</v>
       </c>
     </row>
     <row r="41">
@@ -937,10 +937,10 @@
         <v>92</v>
       </c>
       <c r="C41" t="n">
-        <v>12219.0</v>
+        <v>1767.0</v>
       </c>
       <c r="D41" t="n">
-        <v>1.13</v>
+        <v>1.08</v>
       </c>
     </row>
     <row r="42">
@@ -951,10 +951,10 @@
         <v>93</v>
       </c>
       <c r="C42" t="n">
-        <v>7138.0</v>
+        <v>1164.0</v>
       </c>
       <c r="D42" t="n">
-        <v>1.11</v>
+        <v>1.07</v>
       </c>
     </row>
     <row r="43">
@@ -965,10 +965,10 @@
         <v>94</v>
       </c>
       <c r="C43" t="n">
-        <v>16664.0</v>
+        <v>1164.0</v>
       </c>
       <c r="D43" t="n">
-        <v>1.11</v>
+        <v>1.07</v>
       </c>
     </row>
     <row r="44">
@@ -979,10 +979,10 @@
         <v>95</v>
       </c>
       <c r="C44" t="n">
-        <v>15783.0</v>
+        <v>2482.0</v>
       </c>
       <c r="D44" t="n">
-        <v>1.11</v>
+        <v>1.07</v>
       </c>
     </row>
     <row r="45">
@@ -993,10 +993,10 @@
         <v>96</v>
       </c>
       <c r="C45" t="n">
-        <v>15788.0</v>
+        <v>1208.0</v>
       </c>
       <c r="D45" t="n">
-        <v>1.11</v>
+        <v>1.04</v>
       </c>
     </row>
     <row r="46">
@@ -1007,10 +1007,10 @@
         <v>97</v>
       </c>
       <c r="C46" t="n">
-        <v>15773.0</v>
+        <v>1567.0</v>
       </c>
       <c r="D46" t="n">
-        <v>1.11</v>
+        <v>0.94</v>
       </c>
     </row>
     <row r="47">
@@ -1021,10 +1021,10 @@
         <v>98</v>
       </c>
       <c r="C47" t="n">
-        <v>12211.0</v>
+        <v>1169.0</v>
       </c>
       <c r="D47" t="n">
-        <v>1.11</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="48">
@@ -1035,10 +1035,10 @@
         <v>99</v>
       </c>
       <c r="C48" t="n">
-        <v>9560.0</v>
+        <v>1098.0</v>
       </c>
       <c r="D48" t="n">
-        <v>1.11</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="49">
@@ -1049,10 +1049,10 @@
         <v>100</v>
       </c>
       <c r="C49" t="n">
-        <v>6355.0</v>
+        <v>1095.0</v>
       </c>
       <c r="D49" t="n">
-        <v>1.02</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="50">
@@ -1063,10 +1063,10 @@
         <v>101</v>
       </c>
       <c r="C50" t="n">
-        <v>8048.0</v>
+        <v>1665.0</v>
       </c>
       <c r="D50" t="n">
-        <v>1.01</v>
+        <v>0.83</v>
       </c>
     </row>
     <row r="51">
@@ -1077,10 +1077,10 @@
         <v>102</v>
       </c>
       <c r="C51" t="n">
-        <v>6017.0</v>
+        <v>1240.0</v>
       </c>
       <c r="D51" t="n">
-        <v>0.91</v>
+        <v>0.63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
OpenFDA ror and prr solutions
</commit_message>
<xml_diff>
--- a/RShinyApps/mydata.xlsx
+++ b/RShinyApps/mydata.xlsx
@@ -12,15 +12,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
-    <t>Term</t>
+    <t>Definition</t>
   </si>
   <si>
-    <t>Count</t>
+    <t>Preferred Term</t>
   </si>
   <si>
-    <t>Count.1</t>
+    <t>Counts for OLMESARTAN MEDOXOMIL</t>
   </si>
   <si>
     <t>PRR</t>
@@ -32,7 +32,10 @@
     <t>1</t>
   </si>
   <si>
-    <t>Please enter a Drug name</t>
+    <t>&lt;a href="http://www.merriam-webster.com/medlineplus/SPRUE-LIKE%20ENTEROPATHY" target="_blank"&gt;Definition&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>SPRUE-LIKE ENTEROPATHY</t>
   </si>
 </sst>
 </file>
@@ -108,17 +111,17 @@
       <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="n">
-        <v>0.0</v>
+      <c r="C2" t="s">
+        <v>7</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0</v>
+        <v>3282.0</v>
       </c>
       <c r="E2" t="n">
-        <v>0.0</v>
+        <v>1463.77</v>
       </c>
       <c r="F2" t="n">
-        <v>0.0</v>
+        <v>348.69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>